<commit_message>
Separate tichonov method to another file
</commit_message>
<xml_diff>
--- a/matrixAndVector.xlsx
+++ b/matrixAndVector.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaroslav\Desktop\Univer\MMSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9091336E-34A8-4394-B50C-FD15C199D559}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500FDBA8-42B1-403D-94F0-954045735DA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="3465" windowWidth="21600" windowHeight="12855" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +418,8 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.79597430606372699</v>
+        <f xml:space="preserve"> (4 * D2) + (E2 * F2)</f>
+        <v>2.9263951438100344</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -435,7 +436,8 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.18318820884451301</v>
+        <f t="shared" ref="A3:A31" si="0" xml:space="preserve"> (4 * D3) + (E3 * F3)</f>
+        <v>3.4915071110484712</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -452,7 +454,8 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.22181700658984499</v>
+        <f t="shared" si="0"/>
+        <v>3.8556248895623964</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -469,7 +472,8 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.41954455641098298</v>
+        <f t="shared" si="0"/>
+        <v>4.0792138765211146</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -486,7 +490,8 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.27174598444253201</v>
+        <f t="shared" si="0"/>
+        <v>1.4108023058754844</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -503,7 +508,8 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.312555850483477</v>
+        <f t="shared" si="0"/>
+        <v>2.6145087321769878</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -520,7 +526,8 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.30063931620679801</v>
+        <f t="shared" si="0"/>
+        <v>0.8257172807459876</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -537,7 +544,8 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.73652204056270398</v>
+        <f t="shared" si="0"/>
+        <v>3.7518514455163805</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -554,7 +562,8 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0.73762408085167397</v>
+        <f t="shared" si="0"/>
+        <v>0.64337332103110245</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -571,7 +580,8 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1.41798472031951E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.9735203128391459</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -588,7 +598,8 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.97727475245483197</v>
+        <f t="shared" si="0"/>
+        <v>0.55687397893414448</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -605,7 +616,8 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.103198863333091</v>
+        <f t="shared" si="0"/>
+        <v>3.6859523560642788</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -622,7 +634,8 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.55825320654548705</v>
+        <f t="shared" si="0"/>
+        <v>2.4696867242566789</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -639,7 +652,8 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7.4433261528611197E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.311888646245345</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -656,7 +670,8 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>0.64342554332688495</v>
+        <f t="shared" si="0"/>
+        <v>3.4985312000965907</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -673,7 +688,8 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.46875345217995301</v>
+        <f t="shared" si="0"/>
+        <v>0.89873399377311591</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -690,7 +706,8 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>0.23353732842951999</v>
+        <f t="shared" si="0"/>
+        <v>1.9882963272025758</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -707,7 +724,8 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.908611248014495</v>
+        <f t="shared" si="0"/>
+        <v>2.1404864630907543</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -724,7 +742,8 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>0.76455102255567897</v>
+        <f t="shared" si="0"/>
+        <v>3.0590163911524337</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -741,7 +760,8 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>0.90303585003130105</v>
+        <f t="shared" si="0"/>
+        <v>0.76635412966266003</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -758,7 +778,8 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>0.52277684211731001</v>
+        <f t="shared" si="0"/>
+        <v>1.1967823360692638</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -775,7 +796,8 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>0.43300719722174102</v>
+        <f t="shared" si="0"/>
+        <v>0.5837723014016204</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -792,7 +814,8 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4.2913524201139801E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.2654599658408521</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -809,7 +832,8 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9.3952461844310206E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.56800607394605962</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -826,7 +850,8 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.118186530424282</v>
+        <f t="shared" si="0"/>
+        <v>3.3373462858603506</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -843,7 +868,8 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.15881663281470501</v>
+        <f t="shared" si="0"/>
+        <v>0.68004898798955926</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -860,7 +886,8 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>0.43562472611665698</v>
+        <f t="shared" si="0"/>
+        <v>3.6794751011059397</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -877,7 +904,8 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>0.90774453408084799</v>
+        <f t="shared" si="0"/>
+        <v>2.0552053635047463</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -894,7 +922,8 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>8.0239890841767206E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.65616244067325202</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -911,7 +940,8 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>0.60381257929839205</v>
+        <f t="shared" si="0"/>
+        <v>0.21034497282138823</v>
       </c>
       <c r="C31">
         <v>1</v>

</xml_diff>

<commit_message>
Add squared and linear graphics
</commit_message>
<xml_diff>
--- a/matrixAndVector.xlsx
+++ b/matrixAndVector.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yaroslav\Desktop\Univer\MMSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500FDBA8-42B1-403D-94F0-954045735DA3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F1EB41-1F5A-4AE0-A47E-A54560A9DD39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Vector</t>
+  </si>
+  <si>
+    <t>Vector2</t>
   </si>
 </sst>
 </file>
@@ -95,16 +98,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>142705</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>114262</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152230</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104737</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -127,7 +130,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4876800" y="762000"/>
+          <a:off x="9153525" y="180975"/>
           <a:ext cx="1361905" cy="304762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -403,20 +406,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19:Q48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <f xml:space="preserve"> (4 * D2) + (E2 * F2)</f>
         <v>2.9263951438100344</v>
@@ -433,8 +439,24 @@
       <c r="F2">
         <v>0.58502862602472305</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f xml:space="preserve"> (4 * K2) + (L2 + M2)</f>
+        <v>2.8209005754906697</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.57651667553000197</v>
+      </c>
+      <c r="L2">
+        <v>0.33684131945483398</v>
+      </c>
+      <c r="M2">
+        <v>0.17799255391582799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ref="A3:A31" si="0" xml:space="preserve"> (4 * D3) + (E3 * F3)</f>
         <v>3.4915071110484712</v>
@@ -451,8 +473,24 @@
       <c r="F3">
         <v>0.173634463921189</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" ref="H3:H31" si="1" xml:space="preserve"> (4 * K3) + (L3 + M3)</f>
+        <v>3.7770531291607781</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.65583933377638504</v>
+      </c>
+      <c r="L3">
+        <v>0.60141437523998298</v>
+      </c>
+      <c r="M3">
+        <v>0.55228141881525505</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>3.8556248895623964</v>
@@ -469,8 +507,24 @@
       <c r="F4">
         <v>0.65789761557243798</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>2.0018194515723717</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.46770194335840598</v>
+      </c>
+      <c r="L4">
+        <v>9.0099058812484104E-2</v>
+      </c>
+      <c r="M4">
+        <v>4.0912619326263701E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4.0792138765211146</v>
@@ -487,8 +541,24 @@
       <c r="F5">
         <v>0.43454911746084701</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>1.7887901756912461</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.121764174196869</v>
+      </c>
+      <c r="L5">
+        <v>0.41305971168912903</v>
+      </c>
+      <c r="M5">
+        <v>0.88867376721464097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>1.4108023058754844</v>
@@ -505,8 +575,24 @@
       <c r="F6">
         <v>0.51725128036923695</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>3.629126153420656</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.66233580419793703</v>
+      </c>
+      <c r="L6">
+        <v>0.91595442732796095</v>
+      </c>
+      <c r="M6">
+        <v>6.3828509300947203E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>2.6145087321769878</v>
@@ -523,8 +609,24 @@
       <c r="F7">
         <v>0.93483751453459296</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>4.9378330565523356</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0.80168087733909499</v>
+      </c>
+      <c r="L7">
+        <v>0.81928974599577498</v>
+      </c>
+      <c r="M7">
+        <v>0.91181980120018102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>0.8257172807459876</v>
@@ -541,8 +643,24 @@
       <c r="F8">
         <v>0.633871412836015</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>2.2664381524082291</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.26442150399088898</v>
+      </c>
+      <c r="L8">
+        <v>0.63174218428321205</v>
+      </c>
+      <c r="M8">
+        <v>0.577009952161461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>3.7518514455163805</v>
@@ -559,8 +677,24 @@
       <c r="F9">
         <v>0.89440044737420998</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1.4001220618374659</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0.22510470915585801</v>
+      </c>
+      <c r="L9">
+        <v>0.41121273604221598</v>
+      </c>
+      <c r="M9">
+        <v>8.8490489171817899E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>0.64337332103110245</v>
@@ -577,8 +711,24 @@
       <c r="F10">
         <v>0.10200561257079201</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1.117159771732986</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>4.0861944667994997E-2</v>
+      </c>
+      <c r="L10">
+        <v>0.59970169863663603</v>
+      </c>
+      <c r="M10">
+        <v>0.35401029442436999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>1.9735203128391459</v>
@@ -595,8 +745,24 @@
       <c r="F11">
         <v>0.16382583649829</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>2.695875237695871</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.480717715574428</v>
+      </c>
+      <c r="L11">
+        <v>4.0918290615081801E-2</v>
+      </c>
+      <c r="M11">
+        <v>0.73208608478307702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>0.55687397893414448</v>
@@ -613,8 +779,24 @@
       <c r="F12">
         <v>0.75292941392399404</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>4.0404472108930349</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.88376173214055598</v>
+      </c>
+      <c r="L12">
+        <v>3.1818260438740302E-2</v>
+      </c>
+      <c r="M12">
+        <v>0.47358202189207099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>3.6859523560642788</v>
@@ -631,8 +813,24 @@
       <c r="F13">
         <v>3.3370657125487903E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>3.717081452719869</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.56194948428310498</v>
+      </c>
+      <c r="L13">
+        <v>0.52572452020831395</v>
+      </c>
+      <c r="M13">
+        <v>0.94355899537913501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>2.4696867242566789</v>
@@ -649,8 +847,24 @@
       <c r="F14">
         <v>0.48576095537282499</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1.552045054035263</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0.27270459290593901</v>
+      </c>
+      <c r="L14">
+        <v>0.133798244409263</v>
+      </c>
+      <c r="M14">
+        <v>0.32742843800224403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>3.311888646245345</v>
@@ -667,8 +881,24 @@
       <c r="F15">
         <v>0.11996514769270999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>4.0680233964230847</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0.60438859718851701</v>
+      </c>
+      <c r="L15">
+        <v>0.87994712917134199</v>
+      </c>
+      <c r="M15">
+        <v>0.77052187849767495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>3.4985312000965907</v>
@@ -685,8 +915,24 @@
       <c r="F16">
         <v>0.61582275107502904</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>3.2076576403342179</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>0.61634837789460994</v>
+      </c>
+      <c r="L16">
+        <v>0.15736723272129899</v>
+      </c>
+      <c r="M16">
+        <v>0.58489689603447903</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>0.89873399377311591</v>
@@ -703,8 +949,24 @@
       <c r="F17">
         <v>0.186127469176427</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>1.0300543482881035</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>3.9021216332912403E-2</v>
+      </c>
+      <c r="L17">
+        <v>9.2762751504778904E-2</v>
+      </c>
+      <c r="M17">
+        <v>0.78120673145167496</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>1.9882963272025758</v>
@@ -721,8 +983,24 @@
       <c r="F18">
         <v>0.84301689453423001</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>2.348869703477249</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0.328098440077156</v>
+      </c>
+      <c r="L18">
+        <v>0.961461258586496</v>
+      </c>
+      <c r="M18">
+        <v>7.5014684582129093E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>2.1404864630907543</v>
@@ -739,8 +1017,24 @@
       <c r="F19">
         <v>0.77129370463080704</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>2.9573143483139583</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.52356005785986803</v>
+      </c>
+      <c r="L19">
+        <v>0.57521328632719804</v>
+      </c>
+      <c r="M19">
+        <v>0.287860830547288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>3.0590163911524337</v>
@@ -757,8 +1051,24 @@
       <c r="F20">
         <v>0.66213443619199097</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1.2855629785917695</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>9.8133558407425894E-2</v>
+      </c>
+      <c r="L20">
+        <v>0.531935052014887</v>
+      </c>
+      <c r="M20">
+        <v>0.36109369294717902</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>0.76635412966266003</v>
@@ -775,8 +1085,24 @@
       <c r="F21">
         <v>0.826360005419701</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>3.7884582777041942</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0.91571947443298995</v>
+      </c>
+      <c r="L21">
+        <v>1.26368938945234E-2</v>
+      </c>
+      <c r="M21">
+        <v>0.112943486077711</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>1.1967823360692638</v>
@@ -793,8 +1119,24 @@
       <c r="F22">
         <v>2.7210811385884898E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>2.444380309898408</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0.33056355454027703</v>
+      </c>
+      <c r="L22">
+        <v>0.54515452194027603</v>
+      </c>
+      <c r="M22">
+        <v>0.57697156979702402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>0.5837723014016204</v>
@@ -811,8 +1153,24 @@
       <c r="F23">
         <v>7.71396118216217E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>3.3306091576814625</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>0.53805265389382795</v>
+      </c>
+      <c r="L23">
+        <v>0.71745607722550597</v>
+      </c>
+      <c r="M23">
+        <v>0.460942464880645</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>3.2654599658408521</v>
@@ -829,8 +1187,24 @@
       <c r="F24">
         <v>0.68179664690978803</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>4.2763164513744423</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>0.65983362565748405</v>
+      </c>
+      <c r="L24">
+        <v>0.92317332793027196</v>
+      </c>
+      <c r="M24">
+        <v>0.71380862081423402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>0.56800607394605962</v>
@@ -847,8 +1221,24 @@
       <c r="F25">
         <v>0.56792055023834098</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>2.0159127423539753</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0.35649908776395001</v>
+      </c>
+      <c r="L25">
+        <v>0.52003610460087701</v>
+      </c>
+      <c r="M25">
+        <v>6.9880286697298302E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>3.3373462858603506</v>
@@ -865,8 +1255,24 @@
       <c r="F26">
         <v>5.1695448579266702E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>3.4969582487829012</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>0.83879467076621905</v>
+      </c>
+      <c r="L26">
+        <v>0.108314290177077</v>
+      </c>
+      <c r="M26">
+        <v>3.34652755409479E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>0.68004898798955926</v>
@@ -883,8 +1289,24 @@
       <c r="F27">
         <v>0.39723416650667798</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>0.59098102315329049</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>3.4644349943846499E-3</v>
+      </c>
+      <c r="L27">
+        <v>0.52085627452470395</v>
+      </c>
+      <c r="M27">
+        <v>5.6267008651047903E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>3.6794751011059397</v>
@@ -901,8 +1323,24 @@
       <c r="F28">
         <v>2.2651802515611101E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>4.3687728401273507</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0.83434065012261305</v>
+      </c>
+      <c r="L28">
+        <v>0.75709811085835099</v>
+      </c>
+      <c r="M28">
+        <v>0.27431212877854699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>2.0552053635047463</v>
@@ -919,8 +1357,24 @@
       <c r="F29">
         <v>0.52523746481165301</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>1.452718926826492</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>3.8511824561282999E-2</v>
+      </c>
+      <c r="L29">
+        <v>0.43655731109902302</v>
+      </c>
+      <c r="M29">
+        <v>0.86211431748233702</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>0.65616244067325202</v>
@@ -937,8 +1391,24 @@
       <c r="F30">
         <v>0.51087701995857104</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>1.5660399580374349</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0.103429572191089</v>
+      </c>
+      <c r="L30">
+        <v>0.31249494105577502</v>
+      </c>
+      <c r="M30">
+        <v>0.83982672821730397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>0.21034497282138823</v>
@@ -955,9 +1425,26 @@
       <c r="F31">
         <v>0.82927362131886195</v>
       </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>1.3982889347244041</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>0.10599992168135899</v>
+      </c>
+      <c r="L31">
+        <v>0.249228878878057</v>
+      </c>
+      <c r="M31">
+        <v>0.72506036912091099</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>